<commit_message>
Avoiding overwrite of main branch
</commit_message>
<xml_diff>
--- a/Budget draft 1.xlsx
+++ b/Budget draft 1.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB140AB4-9699-4046-A61E-A65188AEB98C}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30F8A54C-38A0-42DB-96DF-4CDCE9E14FF9}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -559,11 +559,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E34F7AC4-19DC-4F74-A243-4C7FEA4BCB22}">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E14" sqref="E14"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -571,9 +571,10 @@
     <col min="1" max="1" width="9.89453125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="32.15625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.62890625" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.62890625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
@@ -584,12 +585,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="8" customFormat="1" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:7" s="8" customFormat="1" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" s="8" t="str">
         <f>Training!A4</f>
         <v>SEM training</v>
@@ -599,15 +600,15 @@
         <v>325</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="C4" s="9"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="B6" t="str">
         <f>Materials!A1</f>
         <v>Laboratory supplies</v>
@@ -617,12 +618,12 @@
         <v>731.87</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="B9" t="str">
         <f>Microscopy!A4</f>
         <v>SEM use, including prep and imaging</v>
@@ -632,7 +633,7 @@
         <v>1896</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="B10" t="str">
         <f>Microscopy!A7</f>
         <v>TEM (full service)</v>
@@ -641,8 +642,12 @@
         <f>Microscopy!E7</f>
         <v>11100</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="G10" s="5">
+        <f>SUM(C3,C9:C10)</f>
+        <v>13321</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="B11" t="str">
         <f>Microscopy!A9</f>
         <v>TEM image analysis (software use)</v>
@@ -652,12 +657,12 @@
         <v>135</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="B14" t="str">
         <f>Personnel!A5</f>
         <v>RA costs</v>
@@ -667,7 +672,7 @@
         <v>41852.199999999997</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="B15" t="str">
         <f>Personnel!A7</f>
         <v>Undergraduate research assistant</v>
@@ -905,7 +910,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1029,7 +1034,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1104,7 +1109,10 @@
       <c r="A5" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="5"/>
+      <c r="B5" s="5">
+        <f>SUM(B3:B4)</f>
+        <v>39265</v>
+      </c>
       <c r="C5" s="5"/>
       <c r="E5" s="5">
         <f>SUM(E3:E4)</f>
@@ -1141,6 +1149,10 @@
       <c r="E7" s="5">
         <f>(B7+C7)*D7</f>
         <v>1509</v>
+      </c>
+      <c r="F7" s="5">
+        <f>E7*2</f>
+        <v>3018</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">

</xml_diff>